<commit_message>
Sprint 2 planning created
</commit_message>
<xml_diff>
--- a/SprintPlanning/Sprint 2/INFO-5139-Sprint 2 Planning Meeting 1.0.xlsx
+++ b/SprintPlanning/Sprint 2/INFO-5139-Sprint 2 Planning Meeting 1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepp\Documents\GitHub\ApplicationProjectGroup1\SprintPlanning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepp\Documents\GitHub\ApplicationProjectGroup1\SprintPlanning\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DC64AC-40FB-4B53-A5C5-459FCF51755D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64EACAF-51C2-490F-9D11-F5DA63FD4E9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9C5D2BF-3AE6-4156-8BB2-695A131DFF04}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>Row #</t>
   </si>
@@ -197,12 +197,6 @@
     <t>Bikov, Aleksei</t>
   </si>
   <si>
-    <t>Sprint Planning Meeting 1</t>
-  </si>
-  <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -261,88 +255,73 @@
     <t>ReactJS additional packages, e.g. axios for http requsts to endpoints.</t>
   </si>
   <si>
-    <t>Everyone should draw their draft of the design for the app and choose the best one on the next meeting.</t>
-  </si>
-  <si>
     <t>Maybe some AWS free tier services</t>
   </si>
   <si>
-    <t>FYF-1</t>
-  </si>
-  <si>
     <t>FYF-2</t>
   </si>
   <si>
-    <t>FYF-10</t>
-  </si>
-  <si>
     <t>FYF-13</t>
   </si>
   <si>
-    <t>FYF-15</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
-    <t>Register in the app</t>
-  </si>
-  <si>
     <t>Edit my profile</t>
   </si>
   <si>
     <t>Fill in details about myself (Name, Gender, Age, College/University, Country of origin etc).</t>
   </si>
   <si>
-    <t>Continue to creating my profile</t>
-  </si>
-  <si>
     <t>Complete creating my profile</t>
   </si>
   <si>
     <t>Maintain the accuracy of my personal</t>
   </si>
   <si>
-    <t>Create a post on my page</t>
-  </si>
-  <si>
-    <t>Share content with my friendlist</t>
-  </si>
-  <si>
-    <t>Fast sign up with google account</t>
-  </si>
-  <si>
-    <t>Faster/easier sign up</t>
-  </si>
-  <si>
-    <t>Login into account</t>
-  </si>
-  <si>
-    <t>Have access to my account</t>
-  </si>
-  <si>
-    <t>Share my current status</t>
-  </si>
-  <si>
-    <t>So people know what I am up to</t>
-  </si>
-  <si>
-    <t>Create a burger menu for mobile view</t>
-  </si>
-  <si>
-    <t>For people coming to site from mobiles</t>
-  </si>
-  <si>
-    <t>FYF-33</t>
-  </si>
-  <si>
-    <t>FYF-34</t>
-  </si>
-  <si>
-    <t>FYF-39</t>
-  </si>
-  <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>FYF-18</t>
+  </si>
+  <si>
+    <t>Create Group Chat</t>
+  </si>
+  <si>
+    <t>Chat with multiple people in one chat</t>
+  </si>
+  <si>
+    <t>FYF-14</t>
+  </si>
+  <si>
+    <t>Reset my password</t>
+  </si>
+  <si>
+    <t>Recover access to my account</t>
+  </si>
+  <si>
+    <t>FYF-4</t>
+  </si>
+  <si>
+    <t>Add another user to friend-list</t>
+  </si>
+  <si>
+    <t>Build my friendlist for faster access</t>
+  </si>
+  <si>
+    <t>FYF-5</t>
+  </si>
+  <si>
+    <t>Write a message to another user</t>
+  </si>
+  <si>
+    <t>Chat with another user</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint Planning Meeting 2</t>
   </si>
 </sst>
 </file>
@@ -565,38 +544,55 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>279622</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>182755</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3" descr="https://cdn.discordapp.com/attachments/914263834678665236/950864545210048572/Capture2314.PNG">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1865B288-2656-417A-9DBA-6BD57037DB85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F97B629-966A-42D6-8C20-6428B5B3D85D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="4838700"/>
-          <a:ext cx="24339772" cy="12755755"/>
+          <a:ext cx="18288000" cy="9239250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -618,8 +614,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F24383E-81C1-48AA-B3CE-0A4651C21888}" name="Table13" displayName="Table13" ref="A4:F12" totalsRowShown="0">
-  <autoFilter ref="A4:F12" xr:uid="{6A4555D3-6CFC-4813-9C18-EEC3122BBE8B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F24383E-81C1-48AA-B3CE-0A4651C21888}" name="Table13" displayName="Table13" ref="A4:F10" totalsRowShown="0">
+  <autoFilter ref="A4:F10" xr:uid="{6A4555D3-6CFC-4813-9C18-EEC3122BBE8B}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6C40B138-5F4F-4627-81B5-6CCFB7600CDB}" name="Row #"/>
     <tableColumn id="2" xr3:uid="{615EA2A2-FE7A-4D9C-9A42-7FA8DC77F155}" name="ID" dataDxfId="5"/>
@@ -946,7 +942,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C5" sqref="C5:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,7 +958,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="18" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1007,15 +1003,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>14</v>
@@ -1076,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A875DEB-4808-4559-B6A0-559BDD9EE661}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1091,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1149,19 +1142,19 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5"/>
@@ -1172,19 +1165,19 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6"/>
@@ -1195,19 +1188,19 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7"/>
@@ -1218,19 +1211,19 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8"/>
@@ -1241,19 +1234,19 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9"/>
@@ -1264,76 +1257,30 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
         <v>47</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>68</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10"/>
       <c r="K10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11"/>
-      <c r="K11"/>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12"/>
-      <c r="K12"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{D5E28F0E-7D6B-453A-BE92-021A9AAE5A60}">
       <formula1>"00, 01, 02, 03, 04, 05, 06, 07, 08, 09"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F12" xr:uid="{06EE48CD-350C-407D-8C90-E0AF6D94DA36}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F10" xr:uid="{06EE48CD-350C-407D-8C90-E0AF6D94DA36}">
       <formula1>"In Progress, On Hold, Testing, Done, Cancelled"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1350,7 +1297,7 @@
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,7 +1319,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1380,7 +1327,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1388,7 +1335,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1396,7 +1343,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1404,7 +1351,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1412,7 +1359,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>